<commit_message>
wip... 231113piu_a `rdinv.py` clean & clear code
</commit_message>
<xml_diff>
--- a/xl2roefact/excel_invoices/Fact _Petrom_11017969.xlsx
+++ b/xl2roefact/excel_invoices/Fact _Petrom_11017969.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -225,6 +225,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -245,52 +246,61 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -373,7 +383,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -470,10 +480,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -548,14 +554,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -586,9 +584,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>474120</xdr:colOff>
+      <xdr:colOff>473760</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>37800</xdr:rowOff>
+      <xdr:rowOff>37440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -602,7 +600,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4739040" y="162000"/>
-          <a:ext cx="1952280" cy="847440"/>
+          <a:ext cx="1951920" cy="847080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -625,10 +623,10 @@
   <dimension ref="A2:M49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.11"/>
@@ -879,7 +877,7 @@
       <c r="M22" s="23"/>
     </row>
     <row r="23" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="24"/>
+      <c r="A23" s="18"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -940,7 +938,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
-      <c r="H28" s="25" t="s">
+      <c r="H28" s="24" t="s">
         <v>28</v>
       </c>
       <c r="J28" s="5"/>
@@ -949,158 +947,158 @@
       <c r="M28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="27" t="s">
+      <c r="C29" s="25"/>
+      <c r="D29" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E29" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F29" s="26" t="s">
+      <c r="F29" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="G29" s="26" t="s">
+      <c r="G29" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="H29" s="26" t="s">
+      <c r="H29" s="25" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
     </row>
     <row r="31" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="28" t="n">
+      <c r="A31" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="29"/>
-      <c r="D31" s="30" t="n">
+      <c r="C31" s="28"/>
+      <c r="D31" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="E31" s="31" t="n">
+      <c r="E31" s="30" t="n">
         <v>42756.08</v>
       </c>
-      <c r="F31" s="32" t="n">
+      <c r="F31" s="31" t="n">
         <v>0.19</v>
       </c>
-      <c r="G31" s="31" t="n">
+      <c r="G31" s="30" t="n">
         <f aca="false">E31*D31</f>
         <v>42756.08</v>
       </c>
-      <c r="H31" s="31" t="n">
+      <c r="H31" s="30" t="n">
         <f aca="false">G31*F31</f>
         <v>8123.6552</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="28"/>
-      <c r="B32" s="33" t="s">
+      <c r="A32" s="27"/>
+      <c r="B32" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="33"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="35"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="34"/>
     </row>
     <row r="33" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="28"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="35"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="34"/>
     </row>
     <row r="34" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="28"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="36" t="s">
+      <c r="A34" s="27"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="37" t="n">
+      <c r="G34" s="36" t="n">
         <f aca="false">SUM(G31:G33)</f>
         <v>42756.08</v>
       </c>
-      <c r="H34" s="37" t="n">
+      <c r="H34" s="36" t="n">
         <f aca="false">SUM(H31:H33)</f>
         <v>8123.6552</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="38" t="s">
+      <c r="A35" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="39" t="n">
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="38" t="n">
         <f aca="false">SUM(G34:H34)</f>
         <v>50879.7352</v>
       </c>
-      <c r="H35" s="39"/>
+      <c r="H35" s="38"/>
     </row>
     <row r="36" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="40" t="s">
+      <c r="A36" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39"/>
     </row>
     <row r="37" customFormat="false" ht="10.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="42" t="s">
+      <c r="B39" s="41" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="43" t="s">
+      <c r="A41" s="42" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1108,28 +1106,28 @@
       <c r="A42" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H42" s="44" t="s">
+      <c r="H42" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="I42" s="44"/>
+      <c r="I42" s="43"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H43" s="44" t="s">
+      <c r="H43" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="I43" s="44"/>
+      <c r="I43" s="43"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H44" s="44" t="s">
+      <c r="H44" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="I44" s="44"/>
+      <c r="I44" s="43"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
@@ -1138,7 +1136,7 @@
       <c r="D45" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I45" s="44"/>
+      <c r="I45" s="43"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
@@ -1147,16 +1145,16 @@
       <c r="G46" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H46" s="44" t="s">
+      <c r="H46" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="I46" s="44"/>
+      <c r="I46" s="43"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H47" s="44" t="s">
+      <c r="H47" s="43" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1164,7 +1162,7 @@
       <c r="A48" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H48" s="44" t="s">
+      <c r="H48" s="43" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1172,8 +1170,7 @@
       <c r="A49" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G49" s="45"/>
-      <c r="H49" s="46" t="s">
+      <c r="H49" s="43" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>